<commit_message>
Complete first optimisation tutorial
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mesh Params" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Mesh DP ID</t>
   </si>
@@ -54,6 +55,24 @@
   </si>
   <si>
     <t>Average Temp Out</t>
+  </si>
+  <si>
+    <t>Part 2 Geo</t>
+  </si>
+  <si>
+    <t>DP ID</t>
+  </si>
+  <si>
+    <t>In Dia</t>
+  </si>
+  <si>
+    <t>In 2 Angle</t>
+  </si>
+  <si>
+    <t>Massflow</t>
+  </si>
+  <si>
+    <t>OutTemp Range</t>
   </si>
 </sst>
 </file>
@@ -389,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,4 +589,163 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1500</v>
+      </c>
+      <c r="G5">
+        <v>37.86</v>
+      </c>
+      <c r="H5">
+        <v>9.7046000000000007E-3</v>
+      </c>
+      <c r="I5">
+        <v>300.00200000000001</v>
+      </c>
+      <c r="J5" s="2">
+        <f>(I5-$J$2)/$J$2</f>
+        <v>6.666666666698499E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>-45</v>
+      </c>
+      <c r="F6">
+        <v>1500</v>
+      </c>
+      <c r="G6">
+        <v>53.686999999999998</v>
+      </c>
+      <c r="H6">
+        <v>7.2937000000000002E-3</v>
+      </c>
+      <c r="I6">
+        <v>300.07900000000001</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" ref="J6:J8" si="0">(I6-$J$2)/$J$2</f>
+        <v>2.6333333333335911E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>1.5</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1500</v>
+      </c>
+      <c r="G7">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="H7">
+        <v>4.2419399999999996E-3</v>
+      </c>
+      <c r="I7">
+        <v>299.86599999999999</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="0"/>
+        <v>-4.4666666666671518E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1600</v>
+      </c>
+      <c r="H8">
+        <v>5.6457499999999997E-3</v>
+      </c>
+      <c r="I8">
+        <v>300.00299999999999</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>9.9999999999530091E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>